<commit_message>
Update Excel data file
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/updated.xlsx
+++ b/updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahim/Desktop/yetunde/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C63B94D-B681-484A-9F5A-5FB46D5E5142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11248CA0-DA67-8E4C-8998-25F851878753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="3780" windowWidth="27240" windowHeight="16180" xr2:uid="{9FD3F7A1-4F6F-FC4A-99D2-63B2522064BD}"/>
   </bookViews>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C5A3E3-83CF-8E41-BE14-2666FD4E8612}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2130,7 +2130,7 @@
         <v>19</v>
       </c>
       <c r="N29">
-        <v>1310</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -2438,7 +2438,7 @@
         <v>19</v>
       </c>
       <c r="N36">
-        <v>812</v>
+        <v>949</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>